<commit_message>
refactored dataframe to use enums
</commit_message>
<xml_diff>
--- a/data/raw/chart_of_accounts_mapping.xlsx
+++ b/data/raw/chart_of_accounts_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B983AD49-F02D-4CBE-8212-CFAFC7A39FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A215C6B-93A7-4934-9F35-30CFA97B5659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{AFD3C0A3-8020-4CFF-AE98-8A0A48C760AF}"/>
+    <workbookView xWindow="-37150" yWindow="1910" windowWidth="27100" windowHeight="18360" xr2:uid="{AFD3C0A3-8020-4CFF-AE98-8A0A48C760AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
   <si>
     <t>category</t>
   </si>
@@ -56,27 +56,9 @@
     <t>operating expenses</t>
   </si>
   <si>
-    <t>Fringe</t>
-  </si>
-  <si>
-    <t>Service Center</t>
-  </si>
-  <si>
-    <t>Overhead</t>
-  </si>
-  <si>
-    <t>G&amp;A</t>
-  </si>
-  <si>
-    <t>Unallowable</t>
-  </si>
-  <si>
     <t>other expenses</t>
   </si>
   <si>
-    <t>contract</t>
-  </si>
-  <si>
     <t>current assets</t>
   </si>
   <si>
@@ -86,9 +68,6 @@
     <t>other assets</t>
   </si>
   <si>
-    <t>Liabilities</t>
-  </si>
-  <si>
     <t>current liabilities</t>
   </si>
   <si>
@@ -113,15 +92,6 @@
     <t>accrued expenses</t>
   </si>
   <si>
-    <t>bs_is</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>sub_account</t>
-  </si>
-  <si>
     <t>low</t>
   </si>
   <si>
@@ -131,13 +101,112 @@
     <t>other current liabilities</t>
   </si>
   <si>
-    <t>accrued Expenses</t>
-  </si>
-  <si>
     <t>other long term liabilities</t>
   </si>
   <si>
     <t>other revenue</t>
+  </si>
+  <si>
+    <t>contract revenue</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>distributions</t>
+  </si>
+  <si>
+    <t>owners equity</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>direct labor</t>
+  </si>
+  <si>
+    <t>subcontractors</t>
+  </si>
+  <si>
+    <t>other costs</t>
+  </si>
+  <si>
+    <t>facilities</t>
+  </si>
+  <si>
+    <t>fringe</t>
+  </si>
+  <si>
+    <t>overhead</t>
+  </si>
+  <si>
+    <t>g&amp;a</t>
+  </si>
+  <si>
+    <t>unallowable</t>
+  </si>
+  <si>
+    <t>gsa</t>
+  </si>
+  <si>
+    <t>government</t>
+  </si>
+  <si>
+    <t>cecos</t>
+  </si>
+  <si>
+    <t>pto and 401k</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>utilities</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>labor</t>
+  </si>
+  <si>
+    <t>vehicles</t>
+  </si>
+  <si>
+    <t>consulting</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>is_bs</t>
+  </si>
+  <si>
+    <t>liabilities</t>
+  </si>
+  <si>
+    <t>sub_category3</t>
+  </si>
+  <si>
+    <t>subcategory2</t>
+  </si>
+  <si>
+    <t>subcategory</t>
+  </si>
+  <si>
+    <t>other income</t>
+  </si>
+  <si>
+    <t>normal balance</t>
+  </si>
+  <si>
+    <t>debit</t>
+  </si>
+  <si>
+    <t>credit</t>
   </si>
 </sst>
 </file>
@@ -498,80 +567,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393A8571-B3D9-4C52-B6A9-1535AECC30DF}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11000</v>
       </c>
       <c r="B2">
-        <v>11599</v>
+        <v>11999</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>11600</v>
+        <v>12000</v>
       </c>
       <c r="B3">
         <v>13000</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>14700</v>
       </c>
@@ -579,16 +663,22 @@
         <v>16000</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>17500</v>
       </c>
@@ -596,16 +686,19 @@
         <v>19999</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>20000</v>
       </c>
@@ -613,19 +706,22 @@
         <v>20200</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20300</v>
       </c>
@@ -633,19 +729,22 @@
         <v>20399</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>20400</v>
       </c>
@@ -653,19 +752,22 @@
         <v>20999</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>21000</v>
       </c>
@@ -673,19 +775,22 @@
         <v>21999</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>22000</v>
       </c>
@@ -693,163 +798,570 @@
         <v>24999</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>27000</v>
       </c>
       <c r="B11">
+        <v>27099</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>27100</v>
+      </c>
+      <c r="B12">
+        <v>27599</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>27600</v>
+      </c>
+      <c r="B13">
         <v>28999</v>
       </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>30000</v>
       </c>
-      <c r="B12">
-        <v>31199</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B14">
+        <v>30250</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>34000</v>
-      </c>
-      <c r="B13">
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>30300</v>
+      </c>
+      <c r="B15">
+        <v>30800</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>30900</v>
+      </c>
+      <c r="B16">
+        <v>31100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>34500</v>
+      </c>
+      <c r="B17">
+        <v>34599</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>34600</v>
+      </c>
+      <c r="B18">
         <v>40999</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>41000</v>
+      </c>
+      <c r="B19">
+        <v>41000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>42000</v>
+      </c>
+      <c r="B20">
+        <v>42000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>43000</v>
+      </c>
+      <c r="B21">
+        <v>48000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>50000</v>
+      </c>
+      <c r="B22">
+        <v>50200</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>41000</v>
-      </c>
-      <c r="B14">
-        <v>48000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>50000</v>
-      </c>
-      <c r="B15">
-        <v>55000</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="H22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>50300</v>
+      </c>
+      <c r="B23">
+        <v>50400</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>50600</v>
+      </c>
+      <c r="B24">
+        <v>52600</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>53000</v>
+      </c>
+      <c r="B25">
+        <v>65000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>67000</v>
+      </c>
+      <c r="B26">
+        <v>69000</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>70100</v>
+      </c>
+      <c r="B27">
+        <v>70100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>71000</v>
+      </c>
+      <c r="B28">
+        <v>78500</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>79500</v>
+      </c>
+      <c r="B29">
+        <v>79500</v>
+      </c>
+      <c r="C29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>80000</v>
+      </c>
+      <c r="B30">
+        <v>82000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>83000</v>
+      </c>
+      <c r="B31">
+        <v>85000</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>86000</v>
+      </c>
+      <c r="B32">
+        <v>86000</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>87000</v>
+      </c>
+      <c r="B33">
+        <v>89000</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>90000</v>
+      </c>
+      <c r="B34">
+        <v>95999</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>60000</v>
-      </c>
-      <c r="B16">
-        <v>69000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>70000</v>
-      </c>
-      <c r="B17">
-        <v>79999</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>80000</v>
-      </c>
-      <c r="B18">
-        <v>89999</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>90000</v>
-      </c>
-      <c r="B19">
-        <v>95999</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>10</v>
+      <c r="F34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>96000</v>
+      </c>
+      <c r="B35">
+        <v>96000</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tree structure for BS and IS
</commit_message>
<xml_diff>
--- a/data/raw/chart_of_accounts_mapping.xlsx
+++ b/data/raw/chart_of_accounts_mapping.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Finance-Model\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Finance-Model\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A215C6B-93A7-4934-9F35-30CFA97B5659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE3296B-7DF6-46A1-8F1B-0B878436F02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37150" yWindow="1910" windowWidth="27100" windowHeight="18360" xr2:uid="{AFD3C0A3-8020-4CFF-AE98-8A0A48C760AF}"/>
+    <workbookView xWindow="7920" yWindow="2205" windowWidth="16200" windowHeight="10035" xr2:uid="{AFD3C0A3-8020-4CFF-AE98-8A0A48C760AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
   <si>
     <t>category</t>
   </si>
@@ -62,9 +62,6 @@
     <t>current assets</t>
   </si>
   <si>
-    <t>property and equiptment</t>
-  </si>
-  <si>
     <t>other assets</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>accounts receivable</t>
   </si>
   <si>
-    <t>cash and equivelents</t>
-  </si>
-  <si>
     <t>accounts payable</t>
   </si>
   <si>
@@ -207,6 +201,15 @@
   </si>
   <si>
     <t>credit</t>
+  </si>
+  <si>
+    <t>cash and equivalents</t>
+  </si>
+  <si>
+    <t>property and equipment</t>
+  </si>
+  <si>
+    <t>long term assets</t>
   </si>
 </sst>
 </file>
@@ -570,46 +573,46 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>11000</v>
       </c>
@@ -617,10 +620,10 @@
         <v>11999</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -629,10 +632,10 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>12000</v>
       </c>
@@ -640,10 +643,10 @@
         <v>13000</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
@@ -652,10 +655,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>14700</v>
       </c>
@@ -663,22 +666,22 @@
         <v>16000</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>17500</v>
       </c>
@@ -686,19 +689,22 @@
         <v>19999</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>20000</v>
       </c>
@@ -706,22 +712,22 @@
         <v>20200</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>20300</v>
       </c>
@@ -729,22 +735,22 @@
         <v>20399</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>20400</v>
       </c>
@@ -752,22 +758,22 @@
         <v>20999</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>21000</v>
       </c>
@@ -775,22 +781,22 @@
         <v>21999</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>22000</v>
       </c>
@@ -798,22 +804,22 @@
         <v>24999</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>27000</v>
       </c>
@@ -821,19 +827,19 @@
         <v>27099</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>27100</v>
       </c>
@@ -841,19 +847,19 @@
         <v>27599</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>27600</v>
       </c>
@@ -861,19 +867,19 @@
         <v>28999</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>30000</v>
       </c>
@@ -881,22 +887,22 @@
         <v>30250</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>30300</v>
       </c>
@@ -904,22 +910,22 @@
         <v>30800</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>30900</v>
       </c>
@@ -927,22 +933,22 @@
         <v>31100</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>34500</v>
       </c>
@@ -950,22 +956,22 @@
         <v>34599</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>34600</v>
       </c>
@@ -973,22 +979,22 @@
         <v>40999</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>41000</v>
       </c>
@@ -996,19 +1002,19 @@
         <v>41000</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>42000</v>
       </c>
@@ -1016,19 +1022,19 @@
         <v>42000</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>43000</v>
       </c>
@@ -1036,19 +1042,19 @@
         <v>48000</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>50000</v>
       </c>
@@ -1056,22 +1062,22 @@
         <v>50200</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>50300</v>
       </c>
@@ -1079,22 +1085,22 @@
         <v>50400</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>50600</v>
       </c>
@@ -1102,22 +1108,22 @@
         <v>52600</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>53000</v>
       </c>
@@ -1125,22 +1131,22 @@
         <v>65000</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>67000</v>
       </c>
@@ -1148,22 +1154,22 @@
         <v>69000</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>70100</v>
       </c>
@@ -1171,22 +1177,22 @@
         <v>70100</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>71000</v>
       </c>
@@ -1194,22 +1200,22 @@
         <v>78500</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>79500</v>
       </c>
@@ -1217,22 +1223,22 @@
         <v>79500</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>80000</v>
       </c>
@@ -1240,22 +1246,22 @@
         <v>82000</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>83000</v>
       </c>
@@ -1263,22 +1269,22 @@
         <v>85000</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E31" t="s">
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>86000</v>
       </c>
@@ -1286,22 +1292,22 @@
         <v>86000</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>87000</v>
       </c>
@@ -1309,22 +1315,22 @@
         <v>89000</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
         <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>90000</v>
       </c>
@@ -1332,19 +1338,19 @@
         <v>95999</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
         <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>96000</v>
       </c>
@@ -1352,16 +1358,16 @@
         <v>96000</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>